<commit_message>
CP1 heights from 1995 found! and added to maintenance.xlsx
</commit_message>
<xml_diff>
--- a/metadata/GCNet_maintenance.xlsx
+++ b/metadata/GCNet_maintenance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/GCNet_SWVF/ancil/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/AWS/GCNET/GC-Net-level-1-data-processing/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E1A96-AA8D-174A-A530-61E1A22FA144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0ABDA1-837A-874A-807B-4E5ED41D9D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="41360" windowHeight="20280" tabRatio="932" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="35840" windowHeight="20280" tabRatio="932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP1" sheetId="1" r:id="rId1"/>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -632,19 +632,48 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>34799</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
+        <v>34842</v>
+      </c>
+      <c r="C2" s="8">
+        <v>269</v>
+      </c>
+      <c r="D2" s="8">
+        <f>C2</f>
+        <v>269</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>220</v>
+      </c>
+      <c r="H2" s="8">
+        <f>G2</f>
+        <v>220</v>
+      </c>
+      <c r="I2" s="8">
+        <v>350</v>
+      </c>
+      <c r="J2" s="8">
+        <f>I2</f>
+        <v>350</v>
+      </c>
+      <c r="K2" s="8">
+        <v>220</v>
+      </c>
+      <c r="L2" s="8">
+        <f>K2</f>
+        <v>220</v>
+      </c>
+      <c r="M2" s="8">
+        <v>347</v>
+      </c>
+      <c r="N2" s="8">
+        <f>M2</f>
+        <v>347</v>
       </c>
       <c r="O2">
         <v>9.1</v>
@@ -3612,7 +3641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SUM heights from 1996 found! and added to maintenance.xlsx
</commit_message>
<xml_diff>
--- a/metadata/GCNet_maintenance.xlsx
+++ b/metadata/GCNet_maintenance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/AWS/GCNET/GC-Net-level-1-data-processing/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0ABDA1-837A-874A-807B-4E5ED41D9D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BBAD53-D3A5-9146-BDA3-FAA5C5A39E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="35840" windowHeight="20280" tabRatio="932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="35840" windowHeight="20280" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -4799,11 +4799,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="G2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4899,6 +4899,34 @@
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>35198.458333333336</v>
+      </c>
+      <c r="G2" s="8">
+        <v>209</v>
+      </c>
+      <c r="H2" s="8">
+        <f>G2</f>
+        <v>209</v>
+      </c>
+      <c r="I2" s="8">
+        <v>348</v>
+      </c>
+      <c r="J2" s="8">
+        <f>I2</f>
+        <v>348</v>
+      </c>
+      <c r="K2" s="8">
+        <v>209</v>
+      </c>
+      <c r="L2" s="8">
+        <f>K2</f>
+        <v>209</v>
+      </c>
+      <c r="M2" s="8">
+        <v>348</v>
+      </c>
+      <c r="N2" s="8">
+        <f>M2</f>
+        <v>348</v>
       </c>
       <c r="O2">
         <v>0.1</v>

</xml_diff>

<commit_message>
Major change: Using Jason's C files for 1995-2001
</commit_message>
<xml_diff>
--- a/metadata/GCNet_maintenance.xlsx
+++ b/metadata/GCNet_maintenance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/AWS/GCNET/GC-Net-level-1-data-processing/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bav\OneDrive - Geological survey of Denmark and Greenland\Code\PROMICE\GC-Net-Level-1-data-processing\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BBAD53-D3A5-9146-BDA3-FAA5C5A39E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BBAD53-D3A5-9146-BDA3-FAA5C5A39E0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="35840" windowHeight="20280" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="932" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP1" sheetId="1" r:id="rId1"/>
@@ -539,24 +539,24 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="14" width="17.83203125" customWidth="1"/>
-    <col min="15" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="14" width="17.77734375" customWidth="1"/>
+    <col min="15" max="17" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" customWidth="1"/>
     <col min="19" max="19" width="12" customWidth="1"/>
     <col min="20" max="20" width="10.33203125" customWidth="1"/>
-    <col min="21" max="21" width="7.1640625" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" customWidth="1"/>
-    <col min="23" max="23" width="12.83203125" customWidth="1"/>
+    <col min="21" max="21" width="7.109375" customWidth="1"/>
+    <col min="22" max="22" width="10.77734375" customWidth="1"/>
+    <col min="23" max="23" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -630,7 +630,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>34842</v>
       </c>
@@ -706,7 +706,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>35561</v>
       </c>
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>35945</v>
       </c>
@@ -767,7 +767,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>36017</v>
       </c>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>36305.625</v>
       </c>
@@ -858,7 +858,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>36622</v>
       </c>
@@ -896,7 +896,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>37039</v>
       </c>
@@ -928,7 +928,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>37384</v>
       </c>
@@ -966,7 +966,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>37730.5</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>38457.582638888889</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>38864.582638888889</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>40309.582638888889</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>41761.707638888889</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>-1050</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>35945</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>36305.625</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>-160</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>42491</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>42880</v>
       </c>
@@ -1226,9 +1226,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>35065.416666666664</v>
       </c>
@@ -1335,12 +1335,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="15" max="15" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>41848</v>
       </c>
@@ -1462,14 +1462,14 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>39937.5</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>40314</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>40413.833333333336</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>40638</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>41031</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>41392.75</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>41853.583333333336</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>42128.791666666664</v>
       </c>
@@ -1927,12 +1927,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>37048.666666666664</v>
       </c>
@@ -2024,12 +2024,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>35521.875</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>35904.875</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>37047.875</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>37742</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>-600</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>40299</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>-650</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>41415.666666666664</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>42144.666666666664</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>-205</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>42516</v>
       </c>
@@ -2318,12 +2318,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>37048.666666666664</v>
       </c>
@@ -2415,12 +2415,12 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>37048.666666666664</v>
       </c>
@@ -2512,9 +2512,9 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>37048.666666666664</v>
       </c>
@@ -2606,12 +2606,12 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2685,12 +2685,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>37048.666666666664</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>38497</v>
       </c>
@@ -2717,9 +2717,9 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>41740.458333333336</v>
       </c>
@@ -2841,12 +2841,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="19.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2920,12 +2920,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>35551</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>35945</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>36308</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>36680</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>37040</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>40327</v>
       </c>
@@ -3083,12 +3083,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3162,12 +3162,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>35222.666666666664</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>37048.666666666664</v>
       </c>
@@ -3185,13 +3185,13 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>39183.458333333336</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>40039.416666666664</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>41162.416666666664</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>40330</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>40402</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>40544</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>40787</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>40725</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>41153</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>41030</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>41157</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>41455</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>41516</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>42186</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>41883</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>42248</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>42614</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>42979</v>
       </c>
@@ -3518,12 +3518,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>39183.458333333336</v>
       </c>
@@ -3645,27 +3645,27 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="23.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" customWidth="1"/>
-    <col min="16" max="16" width="17.5" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.109375" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
     <col min="17" max="17" width="19.33203125" customWidth="1"/>
-    <col min="18" max="18" width="17.5" customWidth="1"/>
+    <col min="18" max="18" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>35231</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>9.32</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>35538</v>
       </c>
@@ -3839,7 +3839,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>35584</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>35912</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>182.5</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>35913</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>36267</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>212.5</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>36658.5</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>37057.541666666664</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>37396</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>37750</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>38139</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>-75</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>41784.666666666664</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>-600</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>42125</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>42880</v>
       </c>
@@ -4234,16 +4234,16 @@
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" customWidth="1"/>
     <col min="6" max="9" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>35909.832638888889</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>36271.041666666664</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>37048.666666666664</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>37394.5</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>37751</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>38147.541666666664</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>38499.583333333336</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>39268.791666666664</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>-1330</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>39270.5</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>39814</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>-150</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>40298.958333333336</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>41784.832638888889</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>-505</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>42512</v>
       </c>
@@ -4803,26 +4803,26 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="G2:N2"/>
+      <selection pane="bottomRight" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="13" width="6.83203125" customWidth="1"/>
+    <col min="11" max="13" width="6.77734375" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>35198.458333333336</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>35458.375</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>36288.791666666664</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>36289</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>36678</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>37052.447916666664</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>37773</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>38086.416666666664</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -5254,14 +5254,14 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>35554.958333333336</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>36300.746527777781</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>37050.541666666664</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>37771.819444444445</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>40087.625</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>-450</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>40299.625</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>40678.625</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>9.9999999999999645E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>42139.625</v>
       </c>
@@ -5615,14 +5615,14 @@
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>34832.666666666664</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>9.9999999999999645E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>35563.666666666664</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>9.9999999999999645E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>36293.666666666664</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>37773.791666666664</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>37775.666666666664</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>-800</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>38497.020833333336</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>38833.020833333336</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>39923.666666666664</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>-470</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>40695.916666666664</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>-158</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>41790</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>-500</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>42019</v>
       </c>
@@ -6003,19 +6003,19 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" customWidth="1"/>
     <col min="9" max="13" width="7" customWidth="1"/>
-    <col min="14" max="14" width="7.1640625" customWidth="1"/>
+    <col min="14" max="14" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>35542.541666666664</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>36272.541666666664</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>37016.840277777781</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>37742.541666666664</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>38498.833333333336</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>7.46</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>39277.041666666664</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>-340</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>39949.75</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>41784.833333333336</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>42878</v>
       </c>
@@ -6397,24 +6397,24 @@
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" customWidth="1"/>
     <col min="11" max="11" width="6.6640625" customWidth="1"/>
-    <col min="12" max="12" width="7.1640625" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" customWidth="1"/>
     <col min="13" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="17" width="8.1640625" customWidth="1"/>
+    <col min="16" max="17" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>34839.8125</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>35570.8125</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>36300.8125</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>37050.78125</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>37774.8125</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>38276.708333333336</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>42153</v>
       </c>

</xml_diff>